<commit_message>
memory architecture exercise done
</commit_message>
<xml_diff>
--- a/matrix_mult/150244761_solutions.xlsx
+++ b/matrix_mult/150244761_solutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\high-level-synthesis\repo\matrix_mult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFA7E09-477F-46CB-9FBE-90F9B955AF5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB38E8A-08EF-4C6C-8405-33EDE5C6590F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{31898B9F-48B0-4C1C-8BBC-3C2D5AB45A87}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
   <si>
     <t>Throughput</t>
   </si>
@@ -247,7 +247,19 @@
     <t>Wire type interface for comparison</t>
   </si>
   <si>
-    <t>Sol</t>
+    <t>Solution 33: BRAM internal arrays</t>
+  </si>
+  <si>
+    <t>Main, MULT_I II=8</t>
+  </si>
+  <si>
+    <t>All the rest</t>
+  </si>
+  <si>
+    <t>Set transpose in intialization</t>
+  </si>
+  <si>
+    <t>Internal arrays mapped to registers</t>
   </si>
 </sst>
 </file>
@@ -599,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F07A60-64A0-473B-995E-297D1078EF5D}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +686,7 @@
         <v>21</v>
       </c>
       <c r="H5">
-        <f>B5*C5</f>
+        <f t="shared" ref="H5:H27" si="0">B5*C5</f>
         <v>182692527</v>
       </c>
       <c r="I5">
@@ -699,11 +711,11 @@
         <v>21</v>
       </c>
       <c r="H6">
-        <f>B6*C6</f>
+        <f t="shared" si="0"/>
         <v>246828085.20000002</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I23" si="0">H6/MIN($H$5:$H$110)</f>
+        <f t="shared" ref="I6:I23" si="1">H6/MIN($H$5:$H$110)</f>
         <v>783.50909027422881</v>
       </c>
     </row>
@@ -724,11 +736,11 @@
         <v>21</v>
       </c>
       <c r="H7">
-        <f>B7*C7</f>
+        <f t="shared" si="0"/>
         <v>4408381.4400000004</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.993573417050495</v>
       </c>
     </row>
@@ -749,11 +761,11 @@
         <v>22</v>
       </c>
       <c r="H8">
-        <f>B8*C8</f>
+        <f t="shared" si="0"/>
         <v>10942469.119999999</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34.734799399420368</v>
       </c>
     </row>
@@ -774,11 +786,11 @@
         <v>23</v>
       </c>
       <c r="H9">
-        <f>B9*C9</f>
+        <f t="shared" si="0"/>
         <v>14375751.68</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45.633105777563337</v>
       </c>
     </row>
@@ -799,11 +811,11 @@
         <v>24</v>
       </c>
       <c r="H10">
-        <f>B10*C10</f>
+        <f t="shared" si="0"/>
         <v>11826940.16</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.542385494668743</v>
       </c>
     </row>
@@ -824,11 +836,11 @@
         <v>25</v>
       </c>
       <c r="H11">
-        <f>B11*C11</f>
+        <f t="shared" si="0"/>
         <v>1033789.4</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2815689984096701</v>
       </c>
     </row>
@@ -852,11 +864,11 @@
         <v>26</v>
       </c>
       <c r="H12">
-        <f>B12*C12</f>
+        <f t="shared" si="0"/>
         <v>60005277.200000003</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>190.47540766088201</v>
       </c>
     </row>
@@ -877,11 +889,11 @@
         <v>25</v>
       </c>
       <c r="H13">
-        <f>B13*C13</f>
+        <f t="shared" si="0"/>
         <v>1033789.4</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2815689984096701</v>
       </c>
     </row>
@@ -905,11 +917,11 @@
         <v>27</v>
       </c>
       <c r="H14">
-        <f>B14*C14</f>
+        <f t="shared" si="0"/>
         <v>24251989.740000002</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>76.983356262439344</v>
       </c>
     </row>
@@ -933,11 +945,11 @@
         <v>28</v>
       </c>
       <c r="H15">
-        <f>B15*C15</f>
+        <f t="shared" si="0"/>
         <v>2527745.08</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.0238488520104507</v>
       </c>
     </row>
@@ -958,11 +970,11 @@
         <v>21</v>
       </c>
       <c r="H16">
-        <f>B16*C16</f>
+        <f t="shared" si="0"/>
         <v>1553192.76</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9303167644883485</v>
       </c>
     </row>
@@ -983,11 +995,11 @@
         <v>21</v>
       </c>
       <c r="H17">
-        <f>B17*C17</f>
+        <f t="shared" si="0"/>
         <v>1271982.0800000001</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.037666627516832</v>
       </c>
     </row>
@@ -1008,11 +1020,11 @@
         <v>34</v>
       </c>
       <c r="H18">
-        <f>B18*C18</f>
+        <f t="shared" si="0"/>
         <v>513792</v>
       </c>
       <c r="I18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6309355646623009</v>
       </c>
     </row>
@@ -1033,11 +1045,11 @@
         <v>35</v>
       </c>
       <c r="H19">
-        <f>B19*C19</f>
+        <f t="shared" si="0"/>
         <v>336792</v>
       </c>
       <c r="I19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0690825289100367</v>
       </c>
     </row>
@@ -1058,11 +1070,11 @@
         <v>41</v>
       </c>
       <c r="H20">
-        <f>B20*C20</f>
+        <f t="shared" si="0"/>
         <v>315029</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1086,11 +1098,11 @@
         <v>43</v>
       </c>
       <c r="H21">
-        <f>B21*C21</f>
+        <f t="shared" si="0"/>
         <v>7331148</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23.27134327315898</v>
       </c>
     </row>
@@ -1114,11 +1126,11 @@
         <v>44</v>
       </c>
       <c r="H22">
-        <f>B22*C22</f>
+        <f t="shared" si="0"/>
         <v>4154386</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.187312914049183</v>
       </c>
     </row>
@@ -1139,11 +1151,11 @@
         <v>21</v>
       </c>
       <c r="H23">
-        <f>B23*C23</f>
+        <f t="shared" si="0"/>
         <v>4763033.5999999996</v>
       </c>
       <c r="I23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.119349647175339</v>
       </c>
     </row>
@@ -1167,11 +1179,11 @@
         <v>47</v>
       </c>
       <c r="H24">
-        <f>B24*C24</f>
+        <f t="shared" si="0"/>
         <v>354992</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:I27" si="1">H24/MIN($H$5:$H$110)</f>
+        <f t="shared" ref="I24:I27" si="2">H24/MIN($H$5:$H$110)</f>
         <v>1.1268549879534899</v>
       </c>
     </row>
@@ -1198,11 +1210,11 @@
         <v>53</v>
       </c>
       <c r="H25">
-        <f>B25*C25</f>
+        <f t="shared" si="0"/>
         <v>4367616</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.864171235029156</v>
       </c>
     </row>
@@ -1226,11 +1238,11 @@
         <v>65</v>
       </c>
       <c r="H26">
-        <f>B26*C26</f>
+        <f t="shared" si="0"/>
         <v>369984</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1744442575128005</v>
       </c>
     </row>
@@ -1257,11 +1269,11 @@
         <v>68</v>
       </c>
       <c r="H27">
-        <f>B27*C27</f>
+        <f t="shared" si="0"/>
         <v>369816</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1739109732754762</v>
       </c>
     </row>
@@ -1288,11 +1300,11 @@
         <v>67</v>
       </c>
       <c r="H28">
-        <f t="shared" ref="H28:H38" si="2">B28*C28</f>
+        <f t="shared" ref="H28:H33" si="3">B28*C28</f>
         <v>369816</v>
       </c>
       <c r="I28">
-        <f t="shared" ref="I28:I38" si="3">H28/MIN($H$5:$H$110)</f>
+        <f t="shared" ref="I28:I33" si="4">H28/MIN($H$5:$H$110)</f>
         <v>1.1739109732754762</v>
       </c>
     </row>
@@ -1319,11 +1331,11 @@
         <v>63</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>369816</v>
       </c>
       <c r="I29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1739109732754762</v>
       </c>
     </row>
@@ -1350,11 +1362,11 @@
         <v>63</v>
       </c>
       <c r="H30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>369984</v>
       </c>
       <c r="I30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.1744442575128005</v>
       </c>
     </row>
@@ -1381,11 +1393,11 @@
         <v>63</v>
       </c>
       <c r="H31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1863817.2</v>
       </c>
       <c r="I31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.9163353215100827</v>
       </c>
     </row>
@@ -1412,11 +1424,11 @@
         <v>67</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1904651.52</v>
       </c>
       <c r="I32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.045956150068724</v>
       </c>
     </row>
@@ -1443,11 +1455,11 @@
         <v>67</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>424464</v>
       </c>
       <c r="I33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3473807173307855</v>
       </c>
     </row>
@@ -1474,11 +1486,11 @@
         <v>67</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34" si="4">B34*C34</f>
+        <f t="shared" ref="H34" si="5">B34*C34</f>
         <v>1256476.48</v>
       </c>
       <c r="I34">
-        <f t="shared" ref="I34" si="5">H34/MIN($H$5:$H$110)</f>
+        <f t="shared" ref="I34" si="6">H34/MIN($H$5:$H$110)</f>
         <v>3.9884470318605589</v>
       </c>
     </row>
@@ -1505,17 +1517,74 @@
         <v>72</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35" si="6">B35*C35</f>
+        <f t="shared" ref="H35:H37" si="7">B35*C35</f>
         <v>2554240.16</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35" si="7">H35/MIN($H$5:$H$110)</f>
+        <f t="shared" ref="I35:I37" si="8">H35/MIN($H$5:$H$110)</f>
         <v>8.1079524742166598</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
+      </c>
+      <c r="B36">
+        <v>64</v>
+      </c>
+      <c r="C36">
+        <v>10817.62</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="7"/>
+        <v>692327.68</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="8"/>
+        <v>2.1976633262334579</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37">
+        <v>64</v>
+      </c>
+      <c r="C37">
+        <v>8839.5400000000009</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="7"/>
+        <v>565730.56000000006</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="8"/>
+        <v>1.7958047036939457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix hierarchy after testing and synthesis
</commit_message>
<xml_diff>
--- a/matrix_mult/150244761_solutions.xlsx
+++ b/matrix_mult/150244761_solutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\high-level-synthesis\repo\matrix_mult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB38E8A-08EF-4C6C-8405-33EDE5C6590F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2817BB7C-ED8C-4A07-81E8-5F6455870847}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{31898B9F-48B0-4C1C-8BBC-3C2D5AB45A87}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="81">
   <si>
     <t>Throughput</t>
   </si>
@@ -260,6 +260,15 @@
   </si>
   <si>
     <t>Internal arrays mapped to registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution 34: Hierarchical </t>
+  </si>
+  <si>
+    <t>Main II=64</t>
+  </si>
+  <si>
+    <t>Hierarchical design task 2</t>
   </si>
 </sst>
 </file>
@@ -611,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F07A60-64A0-473B-995E-297D1078EF5D}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,11 +1526,11 @@
         <v>72</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:H37" si="7">B35*C35</f>
+        <f t="shared" ref="H35:H38" si="7">B35*C35</f>
         <v>2554240.16</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35:I37" si="8">H35/MIN($H$5:$H$110)</f>
+        <f t="shared" ref="I35:I38" si="8">H35/MIN($H$5:$H$110)</f>
         <v>8.1079524742166598</v>
       </c>
     </row>
@@ -1585,6 +1594,37 @@
       <c r="I37">
         <f t="shared" si="8"/>
         <v>1.7958047036939457</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38">
+        <v>64</v>
+      </c>
+      <c r="C38">
+        <v>15653.38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F38" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" t="s">
+        <v>80</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="7"/>
+        <v>1001816.32</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="8"/>
+        <v>3.1800765008935685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>